<commit_message>
se creo la tabla de pedidos y se hizo el form
</commit_message>
<xml_diff>
--- a/velas3.xlsx
+++ b/velas3.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Hoja 2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Hoja 3" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Hoja 2" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="117">
   <si>
     <t xml:space="preserve">enfermedad </t>
   </si>
@@ -308,10 +309,43 @@
     <t xml:space="preserve">Pereza </t>
   </si>
   <si>
+    <t>intencion</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>aroma</t>
+  </si>
+  <si>
+    <t>mensaje</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amor </t>
+  </si>
+  <si>
+    <t>morada</t>
+  </si>
+  <si>
+    <t>lavanda</t>
+  </si>
+  <si>
+    <t>te quiero</t>
+  </si>
+  <si>
     <t>Veladora</t>
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>precio</t>
   </si>
   <si>
     <t>V1</t>
@@ -363,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -377,6 +411,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -390,6 +425,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2070,16 +2109,80 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="5">
+        <v>45724.0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="31.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>109</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="2">
@@ -2087,7 +2190,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
@@ -2095,7 +2198,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4">
@@ -2103,7 +2206,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -2111,7 +2214,7 @@
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
@@ -2119,7 +2222,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7">
@@ -2127,7 +2230,7 @@
         <v>85</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>